<commit_message>
writing into excel sheet
</commit_message>
<xml_diff>
--- a/VytrackTestUsers.xlsx
+++ b/VytrackTestUsers.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3914" uniqueCount="1481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3938" uniqueCount="1481">
   <si>
     <t>username</t>
   </si>
@@ -4466,13 +4466,13 @@
     <t>n/a</t>
   </si>
   <si>
-    <t>Failed</t>
-  </si>
-  <si>
-    <t>Date of execution</t>
-  </si>
-  <si>
-    <t>2020-04-14</t>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>SKIPPED</t>
   </si>
 </sst>
 </file>
@@ -18241,10 +18241,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -18270,10 +18270,7 @@
         <v>303</v>
       </c>
       <c r="F1" t="s">
-        <v>1478</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1479</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -18293,10 +18290,7 @@
         <v>305</v>
       </c>
       <c r="F2" t="s">
-        <v>1477</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -18316,7 +18310,7 @@
         <v>725</v>
       </c>
       <c r="F3" t="s">
-        <v>1477</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -18336,7 +18330,7 @@
         <v>307</v>
       </c>
       <c r="F4" t="s">
-        <v>1477</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -18356,7 +18350,7 @@
         <v>610</v>
       </c>
       <c r="F5" t="s">
-        <v>1477</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -18376,7 +18370,7 @@
         <v>1021</v>
       </c>
       <c r="F6" t="s">
-        <v>1477</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -18396,7 +18390,7 @@
         <v>1274</v>
       </c>
       <c r="F7" t="s">
-        <v>1477</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -18416,7 +18410,7 @@
         <v>337</v>
       </c>
       <c r="F8" t="s">
-        <v>1477</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -18436,7 +18430,7 @@
         <v>796</v>
       </c>
       <c r="F9" t="s">
-        <v>1477</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -18456,7 +18450,7 @@
         <v>644</v>
       </c>
       <c r="F10" t="s">
-        <v>1477</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -18476,7 +18470,7 @@
         <v>586</v>
       </c>
       <c r="F11" t="s">
-        <v>1477</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -18496,7 +18490,7 @@
         <v>1375</v>
       </c>
       <c r="F12" t="s">
-        <v>1477</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -18516,7 +18510,7 @@
         <v>1001</v>
       </c>
       <c r="F13" t="s">
-        <v>1477</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -18536,7 +18530,7 @@
         <v>1378</v>
       </c>
       <c r="F14" t="s">
-        <v>1477</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -18556,7 +18550,7 @@
         <v>1379</v>
       </c>
       <c r="F15" t="s">
-        <v>1477</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -18576,7 +18570,7 @@
         <v>1381</v>
       </c>
       <c r="F16" t="s">
-        <v>1477</v>
+        <v>1480</v>
       </c>
     </row>
   </sheetData>

</xml_diff>